<commit_message>
A1-A20 tasks Stage-1 and Stage-2
</commit_message>
<xml_diff>
--- a/NyseDev/evidence.xlsx
+++ b/NyseDev/evidence.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\4. VALLI Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\0_4. VALLI Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="9" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
   <si>
     <t>TxHash</t>
   </si>
@@ -72,30 +72,6 @@
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -142,6 +118,183 @@
   </si>
   <si>
     <t>VALLI Team</t>
+  </si>
+  <si>
+    <t>4D32CE6AD4A6A9445E816B56C630A4155F543C99C4868B4BC8EBB829142A2411</t>
+  </si>
+  <si>
+    <t>nyseNFT</t>
+  </si>
+  <si>
+    <t>87ABA119CDD9B4564E1E9CA2ACBD5F6130403B56BFEC347263A90C39D5F5BE67</t>
+  </si>
+  <si>
+    <t>nyse1</t>
+  </si>
+  <si>
+    <t>46AFC7160FA2B6AD968E3FE46E557F74B3D173E180CAB87EC45BB7D4842D7ABE</t>
+  </si>
+  <si>
+    <t>nyse2</t>
+  </si>
+  <si>
+    <t>93CCCCF45348D6418690534BC2F97C70ECFAADB56696986B6C4CF733C1E9C0FB</t>
+  </si>
+  <si>
+    <t>nyse3</t>
+  </si>
+  <si>
+    <t>76FD008F2AD64810F55E949DD31D30F9AD5887DBDF0906BD1AB9644ED6B75F5C</t>
+  </si>
+  <si>
+    <t>wasm.juno1f8xhfdfykkfxukchsdqyurgc24factnhwwg5qgq30q34hvgu5haqaugq8l</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>C1C38CDA8288E9B16CAF4AABA8263DB8838A454BCDA860DF47ACECDDFFA5D52B</t>
+  </si>
+  <si>
+    <t>ibc/D8719FD594F8D8AE9A060F62E091AB2A6C65A106A6BC31355D3C452CFF2D5E07</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>37517337D95D612FE32C16F9E004BEA2B29BBBC952BD55DB78654EFA1F8DBF46</t>
+  </si>
+  <si>
+    <t>F3E06C4237D98D55B8F7E8BABA82849BEF95815B862796124A6BA10B637D12AD</t>
+  </si>
+  <si>
+    <t>ibc/CE8E3787C4EBE15C6FFC3AC98941866ADAE4992B4CBC2B518F59B25157051AD9</t>
+  </si>
+  <si>
+    <t>nyse7</t>
+  </si>
+  <si>
+    <t>ibc/2944D14F519EC36258A4D14AA783CE07EE97D92BC3388F3C8C6A8A52B1269426</t>
+  </si>
+  <si>
+    <t>nyse8</t>
+  </si>
+  <si>
+    <t>ibc/71D54B91DD8DDF289F4586E40C578E4170B964CE1EFEBFB5FAF1873A167DD6E9</t>
+  </si>
+  <si>
+    <t>nyse9</t>
+  </si>
+  <si>
+    <t>ibc/AB61E1D8B266923E0C6A743695C46A32AC8C04D0D09E1497B0384CFFF8B72AA0</t>
+  </si>
+  <si>
+    <t>nyse10</t>
+  </si>
+  <si>
+    <t>ibc/086B4E39299C9098EE3800651ADB1E717222D9D380CB213198B8EC2E95EA61F0</t>
+  </si>
+  <si>
+    <t>nyse11</t>
+  </si>
+  <si>
+    <t>ibc/BA1A25FA0132EF591B8619EC89B019A24E17F1F128BFE07EEA6CA4E24BB17493</t>
+  </si>
+  <si>
+    <t>nyse12</t>
+  </si>
+  <si>
+    <t>DA8C795BE6DD6CC1E5F1C0FE8F33B9A50D3DABB420EE0EB2B2D7E925D28C82F4</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>194D050F9A67C895BE9A7FBE99F03F737F9CAA9B2529BC05B8DB9A3A92E6C622</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>1E5E3C5946AEC3B212DA76C42CCFB3F4C475BB22957077F3A49560C9937061CD</t>
+  </si>
+  <si>
+    <t>E8684151B1F4A6A762B13FD0FD5B58B525C199ABA300B96D4B43F6B63590B1B6</t>
+  </si>
+  <si>
+    <t>9527D812A16982C1CA584C98DDF588C6160B7398B6263B3991C6CD156DE7617E</t>
+  </si>
+  <si>
+    <t>B6838F932760BE373F39F1DA45861D036FCE67F99950F43E1DDFD70DE775AA8C</t>
+  </si>
+  <si>
+    <t>55B6C7BD5FB1F32A624C5B802510F9912C1CE73893B845B0DF616F73388FF84E</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>B8773720631694485A593F68411D8CF6C949F4CC789BCD2BDD1540FFD6B5295D</t>
+  </si>
+  <si>
+    <t>74DD376360A1870D38A24FC65122FD984698359DF5E22CE354B4E9F50FC2AA91</t>
+  </si>
+  <si>
+    <t>4FED626C894CE4F0D547EE22270D1D733377AEC3996A56462727A0C3A4252B09</t>
+  </si>
+  <si>
+    <t>310CBCAF45FD17490FEC34278F4A7288B52BF0406C40D99077D7E666A9E98485</t>
+  </si>
+  <si>
+    <t>FD9AD640D0AD650B04A5BD7DF4332D264CE09FA1415BCD86B33757FA5F994A68</t>
+  </si>
+  <si>
+    <t>494533017C5ABD6FDB4BA582CE9265B888394A9C1D5DD1CC203056D2F62B2E83</t>
+  </si>
+  <si>
+    <t>61C4B6894058FCCC8A3A19972065E4C7CFD07C9B71F79D42D47729FA1EFF7C55</t>
+  </si>
+  <si>
+    <t>5BAF39ABB07E9C5B6FD969317B6D1C2A7EE921B2D2275D46154B933C17884867</t>
+  </si>
+  <si>
+    <t>481615A8020D06114E7D8D6D2D0DAF942513DBB2DCA33E1F4305D1CCDEAC3707</t>
+  </si>
+  <si>
+    <t>288DCFCC888CEFE3CA4DC9BF4B8682EE01B547F42BBCE09BC7B35E90D01824E9</t>
+  </si>
+  <si>
+    <t>49F8E5E4C3BB87D95DEBAF9D5946591A86B325A7B4696A77E3DACDF3375AE9E0</t>
+  </si>
+  <si>
+    <t>FD8BDB683D12E10631AFCC86A95A7E7775CDE2C0CDC86121C570445006A37DE3</t>
+  </si>
+  <si>
+    <t>10CF3C01F4C6F415A19BE466D3561DD7A429FC2FFB542619B8FFEEAC4F26F428</t>
+  </si>
+  <si>
+    <t>553564DB4D93C8C16E873B7C501C26250F4A8B861EBC8D0E01EAF8205FC14D04</t>
+  </si>
+  <si>
+    <t>07AAA0210E26FBED0E30AD30C5CA10C6A50018F97A1161359742EACE9E1E095F</t>
+  </si>
+  <si>
+    <t>70F5B1ACEBC8EB3046B5F758F0710B86516B5D3D386BA9B8481D5101110AC21E</t>
+  </si>
+  <si>
+    <t>28797F3868CC804F598B780122442ED2F10975B2CE677212879E354681D2B5C3</t>
+  </si>
+  <si>
+    <t>E8DD8EE581E64F16072445A377CA055C39F720BFBC3E74F8C65A285D5930AC7E</t>
+  </si>
+  <si>
+    <t>C69420F44097DB9A093A88CAB3666F4DDE0BB18576D2445DD394D3EDBE0E4618</t>
+  </si>
+  <si>
+    <t>0F87ABE94E6347A8A33C74E43BA20EDDD9632BFDD239FCE9CD2F98C95AF7132E</t>
+  </si>
+  <si>
+    <t>A43EB954B317A2BBAD53CE5641E84B654A81AB8137CB2B93BD9F2D65871C030D</t>
   </si>
 </sst>
 </file>
@@ -538,8 +691,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,54 +709,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +772,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -637,10 +792,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +810,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -673,10 +830,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +848,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -709,10 +868,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +886,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -745,10 +906,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -757,6 +918,130 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -804,7 +1089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -852,14 +1137,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -877,37 +1164,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>66</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -925,37 +1226,89 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>70</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -973,37 +1326,67 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1021,154 +1404,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,9 +1596,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1339,13 +1621,35 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1664,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1385,16 +1691,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1715,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1434,16 +1742,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1458,7 +1766,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1483,16 +1793,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1817,9 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1533,16 +1845,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +1869,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1575,14 +1889,15 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1593,7 +1908,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1611,10 +1928,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new tasks in Stage-1
</commit_message>
<xml_diff>
--- a/NyseDev/evidence.xlsx
+++ b/NyseDev/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="9" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,15 +57,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
@@ -295,6 +286,30 @@
   </si>
   <si>
     <t>A43EB954B317A2BBAD53CE5641E84B654A81AB8137CB2B93BD9F2D65871C030D</t>
+  </si>
+  <si>
+    <t>9CEB4243F3D23430427D0C9C5F10AD885A2BFFF7E883E02BA73E1ECC4DFA3F7D</t>
+  </si>
+  <si>
+    <t>C4AE1D47708A70A3289F2B9B7531D20E521F4C24B82B5043236DF9FF4B54E622</t>
+  </si>
+  <si>
+    <t>BD02C37977B65E478EC01F7F19401ABE700BDD1F80FAB969FD8BBBF4BF6370C7</t>
+  </si>
+  <si>
+    <t>66D8DBE2DB54C35D85C8CC00ECCAE81D4FC001AB7D81250EF34507459D3460E3</t>
+  </si>
+  <si>
+    <t>98EF9983F65450D4BB31931D3428BB31F5A0528E0C4C764D6F18D9F15BA124D4</t>
+  </si>
+  <si>
+    <t>30E29EBA6BD9CFC79EFC05168DA9922CB3EDCE1CDB59C2277F9479443538380F</t>
+  </si>
+  <si>
+    <t>0E7F794F454EC18055A87910CD225C3D6A6531795F4C80621B0B6E1916571C64</t>
+  </si>
+  <si>
+    <t>A37D58F75CF7928DA7035A7D32A3D28FBE16F5B1F3F6FF31D4809B2CBF9713B3</t>
   </si>
 </sst>
 </file>
@@ -691,8 +706,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,54 +724,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -784,18 +799,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -822,18 +837,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -860,18 +875,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -898,18 +913,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -944,34 +959,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1006,34 +1021,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1046,9 +1061,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1066,26 +1083,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1094,9 +1124,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1114,23 +1146,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,23 +1208,85 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>35</v>
@@ -1188,23 +1294,61 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1226,80 +1370,58 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1326,128 +1448,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1613,43 +1657,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1680,10 +1724,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1691,16 +1735,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1731,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1742,16 +1786,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1782,10 +1826,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1793,16 +1837,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1834,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1845,16 +1889,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1881,18 +1925,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1920,18 +1964,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>